<commit_message>
FInal nonparametric filter push
</commit_message>
<xml_diff>
--- a/Nonparametric_Filtering/results/results.xlsx
+++ b/Nonparametric_Filtering/results/results.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/paulcrann/Desktop/RBE 595 Advanced Robotic Navigation/Advanced-Robotic-Navigation/Nonparametric_Filtering/results/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{511700B3-3BB5-DB44-AED1-D97CC9F08812}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A95DECBC-9FFC-A64D-92AF-350C2389033C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="380" yWindow="500" windowWidth="28040" windowHeight="16560" xr2:uid="{C5F503F9-1A9D-D443-A757-57F1B0684348}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="8">
   <si>
     <t xml:space="preserve"> M </t>
   </si>
@@ -58,13 +58,16 @@
   <si>
     <t>Rotation</t>
   </si>
+  <si>
+    <t>UKF RMSE Results</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="168" formatCode="0.000"/>
+    <numFmt numFmtId="164" formatCode="0.000"/>
   </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
@@ -107,18 +110,23 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="168" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="168" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="1" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -433,10 +441,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{256FD652-C5B6-0E47-99C4-811DFCF5A125}">
-  <dimension ref="A1:H58"/>
+  <dimension ref="A1:N58"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="50" workbookViewId="0">
-      <selection activeCell="M16" sqref="M16"/>
+    <sheetView tabSelected="1" zoomScale="140" workbookViewId="0">
+      <selection activeCell="L1" sqref="L1:N9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -449,1508 +457,1589 @@
     <col min="6" max="6" width="8.1640625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="7.6640625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="8.1640625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="7.5" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="7.83203125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="8.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A1" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="2"/>
-      <c r="E1" s="2" t="s">
+      <c r="D1" s="6"/>
+      <c r="E1" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="F1" s="2"/>
-      <c r="G1" s="2" t="s">
+      <c r="F1" s="6"/>
+      <c r="G1" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="H1" s="2"/>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A2" s="1"/>
-      <c r="B2" s="1"/>
-      <c r="C2" s="3" t="s">
+      <c r="H1" s="6"/>
+      <c r="L1" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="M1" s="6"/>
+      <c r="N1" s="6"/>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A2" s="7"/>
+      <c r="B2" s="7"/>
+      <c r="C2" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="D2" s="3" t="s">
+      <c r="D2" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="E2" s="3" t="s">
+      <c r="E2" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="F2" s="3" t="s">
+      <c r="F2" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="G2" s="3" t="s">
+      <c r="G2" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="H2" s="3" t="s">
+      <c r="H2" s="2" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A3" s="4">
+      <c r="L2" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="M2" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="N2" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A3" s="3">
         <v>1</v>
       </c>
-      <c r="B3" s="4">
+      <c r="B3" s="3">
         <v>250</v>
       </c>
-      <c r="C3" s="5">
+      <c r="C3" s="4">
         <v>0.16500000000000001</v>
       </c>
-      <c r="D3" s="5">
+      <c r="D3" s="4">
         <v>0.17599999999999999</v>
       </c>
-      <c r="E3" s="5">
+      <c r="E3" s="4">
         <v>0.19700000000000001</v>
       </c>
-      <c r="F3" s="5">
+      <c r="F3" s="4">
         <v>0.192</v>
       </c>
-      <c r="G3" s="5">
+      <c r="G3" s="4">
         <v>0.17</v>
       </c>
-      <c r="H3" s="5">
+      <c r="H3" s="4">
         <v>0.17199999999999999</v>
       </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A4" s="4">
+      <c r="L3" s="9">
         <v>1</v>
       </c>
-      <c r="B4" s="4">
+      <c r="M3" s="4">
+        <v>0.13700000000000001</v>
+      </c>
+      <c r="N3" s="4">
+        <v>6.6000000000000003E-2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A4" s="3">
+        <v>1</v>
+      </c>
+      <c r="B4" s="3">
         <v>500</v>
       </c>
-      <c r="C4" s="5">
+      <c r="C4" s="4">
         <v>0.13700000000000001</v>
       </c>
-      <c r="D4" s="5">
+      <c r="D4" s="4">
         <v>9.8000000000000004E-2</v>
       </c>
-      <c r="E4" s="5">
+      <c r="E4" s="4">
         <v>0.152</v>
       </c>
-      <c r="F4" s="5">
+      <c r="F4" s="4">
         <v>0.113</v>
       </c>
-      <c r="G4" s="5">
+      <c r="G4" s="4">
         <v>0.13900000000000001</v>
       </c>
-      <c r="H4" s="5">
+      <c r="H4" s="4">
         <v>8.7999999999999995E-2</v>
       </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A5" s="4">
+      <c r="L4" s="9">
+        <v>2</v>
+      </c>
+      <c r="M4" s="4">
+        <v>0.107</v>
+      </c>
+      <c r="N4" s="4">
+        <v>5.8999999999999997E-2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A5" s="3">
         <v>1</v>
       </c>
-      <c r="B5" s="4">
+      <c r="B5" s="3">
         <v>750</v>
       </c>
-      <c r="C5" s="5">
+      <c r="C5" s="4">
         <v>0.129</v>
       </c>
-      <c r="D5" s="5">
+      <c r="D5" s="4">
         <v>8.1000000000000003E-2</v>
       </c>
-      <c r="E5" s="5">
+      <c r="E5" s="4">
         <v>0.13400000000000001</v>
       </c>
-      <c r="F5" s="5">
+      <c r="F5" s="4">
         <v>9.1999999999999998E-2</v>
       </c>
-      <c r="G5" s="5">
+      <c r="G5" s="4">
         <v>0.13500000000000001</v>
       </c>
-      <c r="H5" s="5">
+      <c r="H5" s="4">
         <v>0.08</v>
       </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A6" s="4">
+      <c r="L5" s="9">
+        <v>3</v>
+      </c>
+      <c r="M5" s="4">
+        <v>9.2999999999999999E-2</v>
+      </c>
+      <c r="N5" s="4">
+        <v>6.9000000000000006E-2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A6" s="3">
         <v>1</v>
       </c>
-      <c r="B6" s="4">
+      <c r="B6" s="3">
         <v>1000</v>
       </c>
-      <c r="C6" s="5">
+      <c r="C6" s="4">
         <v>0.14000000000000001</v>
       </c>
-      <c r="D6" s="5">
+      <c r="D6" s="4">
         <v>8.3000000000000004E-2</v>
       </c>
-      <c r="E6" s="5">
+      <c r="E6" s="4">
         <v>0.154</v>
       </c>
-      <c r="F6" s="5">
+      <c r="F6" s="4">
         <v>9.4E-2</v>
       </c>
-      <c r="G6" s="5">
+      <c r="G6" s="4">
         <v>0.13900000000000001</v>
       </c>
-      <c r="H6" s="5">
+      <c r="H6" s="4">
         <v>0.08</v>
       </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A7" s="4">
+      <c r="L6" s="9">
+        <v>4</v>
+      </c>
+      <c r="M6" s="4">
+        <v>0.11600000000000001</v>
+      </c>
+      <c r="N6" s="4">
+        <v>5.1999999999999998E-2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A7" s="3">
         <v>1</v>
       </c>
-      <c r="B7" s="4">
+      <c r="B7" s="3">
         <v>2000</v>
       </c>
-      <c r="C7" s="5">
+      <c r="C7" s="4">
         <v>0.127</v>
       </c>
-      <c r="D7" s="5">
+      <c r="D7" s="4">
         <v>8.3000000000000004E-2</v>
       </c>
-      <c r="E7" s="5">
+      <c r="E7" s="4">
         <v>0.13</v>
       </c>
-      <c r="F7" s="5">
+      <c r="F7" s="4">
         <v>9.5000000000000001E-2</v>
       </c>
-      <c r="G7" s="5">
+      <c r="G7" s="4">
         <v>0.13500000000000001</v>
       </c>
-      <c r="H7" s="5">
+      <c r="H7" s="4">
         <v>8.1000000000000003E-2</v>
       </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A8" s="4">
+      <c r="L7" s="9">
+        <v>5</v>
+      </c>
+      <c r="M7" s="4">
+        <v>0.17799999999999999</v>
+      </c>
+      <c r="N7" s="4">
+        <v>0.13500000000000001</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A8" s="3">
         <v>1</v>
       </c>
-      <c r="B8" s="4">
+      <c r="B8" s="3">
         <v>3000</v>
       </c>
-      <c r="C8" s="5">
+      <c r="C8" s="4">
         <v>0.13400000000000001</v>
       </c>
-      <c r="D8" s="5">
+      <c r="D8" s="4">
         <v>8.3000000000000004E-2</v>
       </c>
-      <c r="E8" s="5">
+      <c r="E8" s="4">
         <v>0.14199999999999999</v>
       </c>
-      <c r="F8" s="5">
+      <c r="F8" s="4">
         <v>9.4E-2</v>
       </c>
-      <c r="G8" s="5">
+      <c r="G8" s="4">
         <v>0.13600000000000001</v>
       </c>
-      <c r="H8" s="5">
+      <c r="H8" s="4">
         <v>0.08</v>
       </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A9" s="4">
+      <c r="L8" s="9">
+        <v>6</v>
+      </c>
+      <c r="M8" s="4">
+        <v>0.124</v>
+      </c>
+      <c r="N8" s="4">
+        <v>0.115</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A9" s="3">
         <v>1</v>
       </c>
-      <c r="B9" s="4">
+      <c r="B9" s="3">
         <v>4000</v>
       </c>
-      <c r="C9" s="5">
+      <c r="C9" s="4">
         <v>0.13400000000000001</v>
       </c>
-      <c r="D9" s="5">
+      <c r="D9" s="4">
         <v>8.3000000000000004E-2</v>
       </c>
-      <c r="E9" s="5">
+      <c r="E9" s="4">
         <v>0.14299999999999999</v>
       </c>
-      <c r="F9" s="5">
+      <c r="F9" s="4">
         <v>9.4E-2</v>
       </c>
-      <c r="G9" s="5">
+      <c r="G9" s="4">
         <v>0.13500000000000001</v>
       </c>
-      <c r="H9" s="5">
+      <c r="H9" s="4">
         <v>0.08</v>
       </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A10" s="4">
+      <c r="L9" s="9">
+        <v>7</v>
+      </c>
+      <c r="M9" s="4">
+        <v>0.154</v>
+      </c>
+      <c r="N9" s="4">
+        <v>0.113</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A10" s="3">
         <v>1</v>
       </c>
-      <c r="B10" s="4">
+      <c r="B10" s="3">
         <v>5000</v>
       </c>
-      <c r="C10" s="5">
+      <c r="C10" s="4">
         <v>0.13100000000000001</v>
       </c>
-      <c r="D10" s="5">
+      <c r="D10" s="4">
         <v>8.4000000000000005E-2</v>
       </c>
-      <c r="E10" s="5">
+      <c r="E10" s="4">
         <v>0.13700000000000001</v>
       </c>
-      <c r="F10" s="5">
+      <c r="F10" s="4">
         <v>9.5000000000000001E-2</v>
       </c>
-      <c r="G10" s="5">
+      <c r="G10" s="4">
         <v>0.13400000000000001</v>
       </c>
-      <c r="H10" s="5">
+      <c r="H10" s="4">
         <v>7.9000000000000001E-2</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A11" s="3">
+    <row r="11" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A11" s="2">
         <v>2</v>
       </c>
-      <c r="B11" s="3">
+      <c r="B11" s="2">
         <v>250</v>
       </c>
-      <c r="C11" s="6">
+      <c r="C11" s="5">
         <v>0.11700000000000001</v>
       </c>
-      <c r="D11" s="6">
+      <c r="D11" s="5">
         <v>0.113</v>
       </c>
-      <c r="E11" s="6">
+      <c r="E11" s="5">
         <v>0.13700000000000001</v>
       </c>
-      <c r="F11" s="6">
+      <c r="F11" s="5">
         <v>0.13200000000000001</v>
       </c>
-      <c r="G11" s="6">
+      <c r="G11" s="5">
         <v>0.127</v>
       </c>
-      <c r="H11" s="6">
+      <c r="H11" s="5">
         <v>0.104</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A12" s="3">
+    <row r="12" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A12" s="2">
         <v>2</v>
       </c>
-      <c r="B12" s="3">
+      <c r="B12" s="2">
         <v>500</v>
       </c>
-      <c r="C12" s="6">
+      <c r="C12" s="5">
         <v>0.11600000000000001</v>
       </c>
-      <c r="D12" s="6">
+      <c r="D12" s="5">
         <v>9.5000000000000001E-2</v>
       </c>
-      <c r="E12" s="6">
+      <c r="E12" s="5">
         <v>0.13</v>
       </c>
-      <c r="F12" s="6">
+      <c r="F12" s="5">
         <v>0.11</v>
       </c>
-      <c r="G12" s="6">
+      <c r="G12" s="5">
         <v>0.129</v>
       </c>
-      <c r="H12" s="6">
+      <c r="H12" s="5">
         <v>9.0999999999999998E-2</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A13" s="3">
+    <row r="13" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A13" s="2">
         <v>2</v>
       </c>
-      <c r="B13" s="3">
+      <c r="B13" s="2">
         <v>750</v>
       </c>
-      <c r="C13" s="6">
+      <c r="C13" s="5">
         <v>0.11600000000000001</v>
       </c>
-      <c r="D13" s="6">
+      <c r="D13" s="5">
         <v>9.2999999999999999E-2</v>
       </c>
-      <c r="E13" s="6">
+      <c r="E13" s="5">
         <v>0.13400000000000001</v>
       </c>
-      <c r="F13" s="6">
+      <c r="F13" s="5">
         <v>0.11</v>
       </c>
-      <c r="G13" s="6">
+      <c r="G13" s="5">
         <v>0.125</v>
       </c>
-      <c r="H13" s="6">
+      <c r="H13" s="5">
         <v>8.5000000000000006E-2</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A14" s="3">
+    <row r="14" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A14" s="2">
         <v>2</v>
       </c>
-      <c r="B14" s="3">
+      <c r="B14" s="2">
         <v>1000</v>
       </c>
-      <c r="C14" s="6">
+      <c r="C14" s="5">
         <v>0.109</v>
       </c>
-      <c r="D14" s="6">
+      <c r="D14" s="5">
         <v>8.5000000000000006E-2</v>
       </c>
-      <c r="E14" s="6">
+      <c r="E14" s="5">
         <v>0.125</v>
       </c>
-      <c r="F14" s="6">
+      <c r="F14" s="5">
         <v>0.10100000000000001</v>
       </c>
-      <c r="G14" s="6">
+      <c r="G14" s="5">
         <v>0.123</v>
       </c>
-      <c r="H14" s="6">
+      <c r="H14" s="5">
         <v>0.08</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A15" s="3">
+    <row r="15" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A15" s="2">
         <v>2</v>
       </c>
-      <c r="B15" s="3">
+      <c r="B15" s="2">
         <v>2000</v>
       </c>
-      <c r="C15" s="6">
+      <c r="C15" s="5">
         <v>0.111</v>
       </c>
-      <c r="D15" s="6">
+      <c r="D15" s="5">
         <v>9.4E-2</v>
       </c>
-      <c r="E15" s="6">
+      <c r="E15" s="5">
         <v>0.125</v>
       </c>
-      <c r="F15" s="6">
+      <c r="F15" s="5">
         <v>0.113</v>
       </c>
-      <c r="G15" s="6">
+      <c r="G15" s="5">
         <v>0.124</v>
       </c>
-      <c r="H15" s="6">
+      <c r="H15" s="5">
         <v>8.6999999999999994E-2</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A16" s="3">
+    <row r="16" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A16" s="2">
         <v>2</v>
       </c>
-      <c r="B16" s="3">
+      <c r="B16" s="2">
         <v>3000</v>
       </c>
-      <c r="C16" s="6">
+      <c r="C16" s="5">
         <v>0.11700000000000001</v>
       </c>
-      <c r="D16" s="6">
+      <c r="D16" s="5">
         <v>0.84</v>
       </c>
-      <c r="E16" s="6">
+      <c r="E16" s="5">
         <v>0.13400000000000001</v>
       </c>
-      <c r="F16" s="6">
+      <c r="F16" s="5">
         <v>9.9000000000000005E-2</v>
       </c>
-      <c r="G16" s="6">
+      <c r="G16" s="5">
         <v>0.127</v>
       </c>
-      <c r="H16" s="6">
+      <c r="H16" s="5">
         <v>7.9000000000000001E-2</v>
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A17" s="3">
+      <c r="A17" s="2">
         <v>2</v>
       </c>
-      <c r="B17" s="3">
+      <c r="B17" s="2">
         <v>4000</v>
       </c>
-      <c r="C17" s="6">
+      <c r="C17" s="5">
         <v>0.115</v>
       </c>
-      <c r="D17" s="6">
+      <c r="D17" s="5">
         <v>8.7999999999999995E-2</v>
       </c>
-      <c r="E17" s="6">
+      <c r="E17" s="5">
         <v>0.13100000000000001</v>
       </c>
-      <c r="F17" s="6">
+      <c r="F17" s="5">
         <v>0.104</v>
       </c>
-      <c r="G17" s="6">
+      <c r="G17" s="5">
         <v>0.123</v>
       </c>
-      <c r="H17" s="6">
+      <c r="H17" s="5">
         <v>8.1000000000000003E-2</v>
       </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A18" s="3">
+      <c r="A18" s="2">
         <v>2</v>
       </c>
-      <c r="B18" s="3">
+      <c r="B18" s="2">
         <v>5000</v>
       </c>
-      <c r="C18" s="6">
+      <c r="C18" s="5">
         <v>0.112</v>
       </c>
-      <c r="D18" s="6">
+      <c r="D18" s="5">
         <v>8.8999999999999996E-2</v>
       </c>
-      <c r="E18" s="6">
+      <c r="E18" s="5">
         <v>0.128</v>
       </c>
-      <c r="F18" s="6">
+      <c r="F18" s="5">
         <v>0.106</v>
       </c>
-      <c r="G18" s="6">
+      <c r="G18" s="5">
         <v>0.121</v>
       </c>
-      <c r="H18" s="6">
+      <c r="H18" s="5">
         <v>0.08</v>
       </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A19" s="4">
+      <c r="A19" s="3">
         <v>3</v>
       </c>
-      <c r="B19" s="4">
+      <c r="B19" s="3">
         <v>250</v>
       </c>
-      <c r="C19" s="5">
+      <c r="C19" s="4">
         <v>0.10100000000000001</v>
       </c>
-      <c r="D19" s="5">
+      <c r="D19" s="4">
         <v>0.12</v>
       </c>
-      <c r="E19" s="5">
+      <c r="E19" s="4">
         <v>0.11600000000000001</v>
       </c>
-      <c r="F19" s="5">
+      <c r="F19" s="4">
         <v>0.13200000000000001</v>
       </c>
-      <c r="G19" s="5">
+      <c r="G19" s="4">
         <v>0.107</v>
       </c>
-      <c r="H19" s="5">
+      <c r="H19" s="4">
         <v>0.11899999999999999</v>
       </c>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A20" s="4">
+      <c r="A20" s="3">
         <v>3</v>
       </c>
-      <c r="B20" s="4">
+      <c r="B20" s="3">
         <v>500</v>
       </c>
-      <c r="C20" s="5">
+      <c r="C20" s="4">
         <v>9.7000000000000003E-2</v>
       </c>
-      <c r="D20" s="5">
+      <c r="D20" s="4">
         <v>9.9000000000000005E-2</v>
       </c>
-      <c r="E20" s="5">
+      <c r="E20" s="4">
         <v>0.107</v>
       </c>
-      <c r="F20" s="5">
+      <c r="F20" s="4">
         <v>0.11</v>
       </c>
-      <c r="G20" s="5">
+      <c r="G20" s="4">
         <v>0.106</v>
       </c>
-      <c r="H20" s="5">
+      <c r="H20" s="4">
         <v>9.6000000000000002E-2</v>
       </c>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A21" s="4">
+      <c r="A21" s="3">
         <v>3</v>
       </c>
-      <c r="B21" s="4">
+      <c r="B21" s="3">
         <v>750</v>
       </c>
-      <c r="C21" s="5">
+      <c r="C21" s="4">
         <v>9.4E-2</v>
       </c>
-      <c r="D21" s="5">
+      <c r="D21" s="4">
         <v>9.1999999999999998E-2</v>
       </c>
-      <c r="E21" s="5">
+      <c r="E21" s="4">
         <v>0.10299999999999999</v>
       </c>
-      <c r="F21" s="5">
+      <c r="F21" s="4">
         <v>0.10299999999999999</v>
       </c>
-      <c r="G21" s="5">
+      <c r="G21" s="4">
         <v>0.104</v>
       </c>
-      <c r="H21" s="5">
+      <c r="H21" s="4">
         <v>9.1999999999999998E-2</v>
       </c>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A22" s="4">
+      <c r="A22" s="3">
         <v>3</v>
       </c>
-      <c r="B22" s="4">
+      <c r="B22" s="3">
         <v>1000</v>
       </c>
-      <c r="C22" s="5">
+      <c r="C22" s="4">
         <v>9.7000000000000003E-2</v>
       </c>
-      <c r="D22" s="5">
+      <c r="D22" s="4">
         <v>0.09</v>
       </c>
-      <c r="E22" s="5">
+      <c r="E22" s="4">
         <v>0.108</v>
       </c>
-      <c r="F22" s="5">
+      <c r="F22" s="4">
         <v>0.1</v>
       </c>
-      <c r="G22" s="5">
+      <c r="G22" s="4">
         <v>0.105</v>
       </c>
-      <c r="H22" s="5">
+      <c r="H22" s="4">
         <v>0.09</v>
       </c>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A23" s="4">
+      <c r="A23" s="3">
         <v>3</v>
       </c>
-      <c r="B23" s="4">
+      <c r="B23" s="3">
         <v>2000</v>
       </c>
-      <c r="C23" s="5">
+      <c r="C23" s="4">
         <v>9.6000000000000002E-2</v>
       </c>
-      <c r="D23" s="5">
+      <c r="D23" s="4">
         <v>9.5000000000000001E-2</v>
       </c>
-      <c r="E23" s="5">
+      <c r="E23" s="4">
         <v>0.104</v>
       </c>
-      <c r="F23" s="5">
+      <c r="F23" s="4">
         <v>0.107</v>
       </c>
-      <c r="G23" s="5">
+      <c r="G23" s="4">
         <v>0.104</v>
       </c>
-      <c r="H23" s="5">
+      <c r="H23" s="4">
         <v>0.09</v>
       </c>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A24" s="4">
+      <c r="A24" s="3">
         <v>3</v>
       </c>
-      <c r="B24" s="4">
+      <c r="B24" s="3">
         <v>3000</v>
       </c>
-      <c r="C24" s="5">
+      <c r="C24" s="4">
         <v>9.1999999999999998E-2</v>
       </c>
-      <c r="D24" s="5">
+      <c r="D24" s="4">
         <v>9.1999999999999998E-2</v>
       </c>
-      <c r="E24" s="5">
+      <c r="E24" s="4">
         <v>9.7000000000000003E-2</v>
       </c>
-      <c r="F24" s="5">
+      <c r="F24" s="4">
         <v>0.104</v>
       </c>
-      <c r="G24" s="5">
+      <c r="G24" s="4">
         <v>0.10199999999999999</v>
       </c>
-      <c r="H24" s="5">
+      <c r="H24" s="4">
         <v>9.0999999999999998E-2</v>
       </c>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A25" s="4">
+      <c r="A25" s="3">
         <v>3</v>
       </c>
-      <c r="B25" s="4">
+      <c r="B25" s="3">
         <v>4000</v>
       </c>
-      <c r="C25" s="5">
+      <c r="C25" s="4">
         <v>9.6000000000000002E-2</v>
       </c>
-      <c r="D25" s="5">
+      <c r="D25" s="4">
         <v>0.88</v>
       </c>
-      <c r="E25" s="5">
+      <c r="E25" s="4">
         <v>0.10299999999999999</v>
       </c>
-      <c r="F25" s="5">
+      <c r="F25" s="4">
         <v>9.8000000000000004E-2</v>
       </c>
-      <c r="G25" s="5">
+      <c r="G25" s="4">
         <v>0.10299999999999999</v>
       </c>
-      <c r="H25" s="5">
+      <c r="H25" s="4">
         <v>8.7999999999999995E-2</v>
       </c>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A26" s="4">
+      <c r="A26" s="3">
         <v>3</v>
       </c>
-      <c r="B26" s="4">
+      <c r="B26" s="3">
         <v>5000</v>
       </c>
-      <c r="C26" s="5">
+      <c r="C26" s="4">
         <v>9.2999999999999999E-2</v>
       </c>
-      <c r="D26" s="5">
+      <c r="D26" s="4">
         <v>8.5999999999999993E-2</v>
       </c>
-      <c r="E26" s="5">
+      <c r="E26" s="4">
         <v>9.9000000000000005E-2</v>
       </c>
-      <c r="F26" s="5">
+      <c r="F26" s="4">
         <v>9.5000000000000001E-2</v>
       </c>
-      <c r="G26" s="5">
+      <c r="G26" s="4">
         <v>0.10199999999999999</v>
       </c>
-      <c r="H26" s="5">
+      <c r="H26" s="4">
         <v>8.6999999999999994E-2</v>
       </c>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A27" s="3">
+      <c r="A27" s="2">
         <v>4</v>
       </c>
-      <c r="B27" s="3">
+      <c r="B27" s="2">
         <v>250</v>
       </c>
-      <c r="C27" s="6">
+      <c r="C27" s="5">
         <v>0.13400000000000001</v>
       </c>
-      <c r="D27" s="6">
+      <c r="D27" s="5">
         <v>0.13600000000000001</v>
       </c>
-      <c r="E27" s="6">
+      <c r="E27" s="5">
         <v>0.159</v>
       </c>
-      <c r="F27" s="6">
+      <c r="F27" s="5">
         <v>0.154</v>
       </c>
-      <c r="G27" s="6">
+      <c r="G27" s="5">
         <v>0.13400000000000001</v>
       </c>
-      <c r="H27" s="6">
+      <c r="H27" s="5">
         <v>0.13100000000000001</v>
       </c>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A28" s="3">
+      <c r="A28" s="2">
         <v>4</v>
       </c>
-      <c r="B28" s="3">
+      <c r="B28" s="2">
         <v>500</v>
       </c>
-      <c r="C28" s="6">
+      <c r="C28" s="5">
         <v>0.11600000000000001</v>
       </c>
-      <c r="D28" s="6">
+      <c r="D28" s="5">
         <v>0.11899999999999999</v>
       </c>
-      <c r="E28" s="6">
+      <c r="E28" s="5">
         <v>0.126</v>
       </c>
-      <c r="F28" s="6">
+      <c r="F28" s="5">
         <v>0.14000000000000001</v>
       </c>
-      <c r="G28" s="6">
+      <c r="G28" s="5">
         <v>0.125</v>
       </c>
-      <c r="H28" s="6">
+      <c r="H28" s="5">
         <v>0.11</v>
       </c>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A29" s="3">
+      <c r="A29" s="2">
         <v>4</v>
       </c>
-      <c r="B29" s="3">
+      <c r="B29" s="2">
         <v>750</v>
       </c>
-      <c r="C29" s="6">
+      <c r="C29" s="5">
         <v>0.123</v>
       </c>
-      <c r="D29" s="6">
+      <c r="D29" s="5">
         <v>0.10199999999999999</v>
       </c>
-      <c r="E29" s="6">
+      <c r="E29" s="5">
         <v>0.14000000000000001</v>
       </c>
-      <c r="F29" s="6">
+      <c r="F29" s="5">
         <v>0.11899999999999999</v>
       </c>
-      <c r="G29" s="6">
+      <c r="G29" s="5">
         <v>0.126</v>
       </c>
-      <c r="H29" s="6">
+      <c r="H29" s="5">
         <v>9.7000000000000003E-2</v>
       </c>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A30" s="3">
+      <c r="A30" s="2">
         <v>4</v>
       </c>
-      <c r="B30" s="3">
+      <c r="B30" s="2">
         <v>1000</v>
       </c>
-      <c r="C30" s="6">
+      <c r="C30" s="5">
         <v>0.11700000000000001</v>
       </c>
-      <c r="D30" s="6">
+      <c r="D30" s="5">
         <v>0.105</v>
       </c>
-      <c r="E30" s="6">
+      <c r="E30" s="5">
         <v>0.128</v>
       </c>
-      <c r="F30" s="6">
+      <c r="F30" s="5">
         <v>0.124</v>
       </c>
-      <c r="G30" s="6">
+      <c r="G30" s="5">
         <v>0.124</v>
       </c>
-      <c r="H30" s="6">
+      <c r="H30" s="5">
         <v>9.8000000000000004E-2</v>
       </c>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A31" s="3">
+      <c r="A31" s="2">
         <v>4</v>
       </c>
-      <c r="B31" s="3">
+      <c r="B31" s="2">
         <v>2000</v>
       </c>
-      <c r="C31" s="6">
+      <c r="C31" s="5">
         <v>0.11600000000000001</v>
       </c>
-      <c r="D31" s="6">
+      <c r="D31" s="5">
         <v>0.10199999999999999</v>
       </c>
-      <c r="E31" s="6">
+      <c r="E31" s="5">
         <v>0.125</v>
       </c>
-      <c r="F31" s="6">
+      <c r="F31" s="5">
         <v>0.11899999999999999</v>
       </c>
-      <c r="G31" s="6">
+      <c r="G31" s="5">
         <v>0.125</v>
       </c>
-      <c r="H31" s="6">
+      <c r="H31" s="5">
         <v>9.6000000000000002E-2</v>
       </c>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A32" s="3">
+      <c r="A32" s="2">
         <v>4</v>
       </c>
-      <c r="B32" s="3">
+      <c r="B32" s="2">
         <v>3000</v>
       </c>
-      <c r="C32" s="6">
+      <c r="C32" s="5">
         <v>0.113</v>
       </c>
-      <c r="D32" s="6">
+      <c r="D32" s="5">
         <v>0.1</v>
       </c>
-      <c r="E32" s="6">
+      <c r="E32" s="5">
         <v>0.11899999999999999</v>
       </c>
-      <c r="F32" s="6">
+      <c r="F32" s="5">
         <v>0.11799999999999999</v>
       </c>
-      <c r="G32" s="6">
+      <c r="G32" s="5">
         <v>0.123</v>
       </c>
-      <c r="H32" s="6">
+      <c r="H32" s="5">
         <v>9.1999999999999998E-2</v>
       </c>
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A33" s="3">
+      <c r="A33" s="2">
         <v>4</v>
       </c>
-      <c r="B33" s="3">
+      <c r="B33" s="2">
         <v>4000</v>
       </c>
-      <c r="C33" s="6">
+      <c r="C33" s="5">
         <v>0.115</v>
       </c>
-      <c r="D33" s="6">
+      <c r="D33" s="5">
         <v>9.8000000000000004E-2</v>
       </c>
-      <c r="E33" s="6">
+      <c r="E33" s="5">
         <v>0.121</v>
       </c>
-      <c r="F33" s="6">
+      <c r="F33" s="5">
         <v>0.11700000000000001</v>
       </c>
-      <c r="G33" s="6">
+      <c r="G33" s="5">
         <v>0.124</v>
       </c>
-      <c r="H33" s="6">
+      <c r="H33" s="5">
         <v>0.09</v>
       </c>
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A34" s="3">
+      <c r="A34" s="2">
         <v>4</v>
       </c>
-      <c r="B34" s="3">
+      <c r="B34" s="2">
         <v>5000</v>
       </c>
-      <c r="C34" s="6">
+      <c r="C34" s="5">
         <v>0.11600000000000001</v>
       </c>
-      <c r="D34" s="6">
+      <c r="D34" s="5">
         <v>9.8000000000000004E-2</v>
       </c>
-      <c r="E34" s="6">
+      <c r="E34" s="5">
         <v>0.123</v>
       </c>
-      <c r="F34" s="6">
+      <c r="F34" s="5">
         <v>0.11600000000000001</v>
       </c>
-      <c r="G34" s="6">
+      <c r="G34" s="5">
         <v>0.123</v>
       </c>
-      <c r="H34" s="6">
+      <c r="H34" s="5">
         <v>9.0999999999999998E-2</v>
       </c>
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A35" s="4">
+      <c r="A35" s="3">
         <v>5</v>
       </c>
-      <c r="B35" s="4">
+      <c r="B35" s="3">
         <v>250</v>
       </c>
-      <c r="C35" s="5">
+      <c r="C35" s="4">
         <v>0.251</v>
       </c>
-      <c r="D35" s="5">
+      <c r="D35" s="4">
         <v>0.14000000000000001</v>
       </c>
-      <c r="E35" s="5">
+      <c r="E35" s="4">
         <v>0.26</v>
       </c>
-      <c r="F35" s="5">
+      <c r="F35" s="4">
         <v>0.13900000000000001</v>
       </c>
-      <c r="G35" s="5">
+      <c r="G35" s="4">
         <v>0.249</v>
       </c>
-      <c r="H35" s="5">
+      <c r="H35" s="4">
         <v>0.14599999999999999</v>
       </c>
     </row>
     <row r="36" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A36" s="4">
+      <c r="A36" s="3">
         <v>5</v>
       </c>
-      <c r="B36" s="4">
+      <c r="B36" s="3">
         <v>500</v>
       </c>
-      <c r="C36" s="5">
+      <c r="C36" s="4">
         <v>0.247</v>
       </c>
-      <c r="D36" s="5">
+      <c r="D36" s="4">
         <v>0.13200000000000001</v>
       </c>
-      <c r="E36" s="5">
+      <c r="E36" s="4">
         <v>0.252</v>
       </c>
-      <c r="F36" s="5">
+      <c r="F36" s="4">
         <v>0.129</v>
       </c>
-      <c r="G36" s="5">
+      <c r="G36" s="4">
         <v>0.247</v>
       </c>
-      <c r="H36" s="5">
+      <c r="H36" s="4">
         <v>0.14399999999999999</v>
       </c>
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A37" s="4">
+      <c r="A37" s="3">
         <v>5</v>
       </c>
-      <c r="B37" s="4">
+      <c r="B37" s="3">
         <v>750</v>
       </c>
-      <c r="C37" s="5">
+      <c r="C37" s="4">
         <v>0.248</v>
       </c>
-      <c r="D37" s="5">
+      <c r="D37" s="4">
         <v>0.13500000000000001</v>
       </c>
-      <c r="E37" s="5">
+      <c r="E37" s="4">
         <v>0.254</v>
       </c>
-      <c r="F37" s="5">
+      <c r="F37" s="4">
         <v>0.13200000000000001</v>
       </c>
-      <c r="G37" s="5">
+      <c r="G37" s="4">
         <v>0.248</v>
       </c>
-      <c r="H37" s="5">
+      <c r="H37" s="4">
         <v>0.14699999999999999</v>
       </c>
     </row>
     <row r="38" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A38" s="4">
+      <c r="A38" s="3">
         <v>5</v>
       </c>
-      <c r="B38" s="4">
+      <c r="B38" s="3">
         <v>1000</v>
       </c>
-      <c r="C38" s="5">
+      <c r="C38" s="4">
         <v>0.252</v>
       </c>
-      <c r="D38" s="5">
+      <c r="D38" s="4">
         <v>0.13800000000000001</v>
       </c>
-      <c r="E38" s="5">
+      <c r="E38" s="4">
         <v>0.26</v>
       </c>
-      <c r="F38" s="5">
+      <c r="F38" s="4">
         <v>0.13700000000000001</v>
       </c>
-      <c r="G38" s="5">
+      <c r="G38" s="4">
         <v>0.251</v>
       </c>
-      <c r="H38" s="5">
+      <c r="H38" s="4">
         <v>0.14000000000000001</v>
       </c>
     </row>
     <row r="39" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A39" s="4">
+      <c r="A39" s="3">
         <v>5</v>
       </c>
-      <c r="B39" s="4">
+      <c r="B39" s="3">
         <v>2000</v>
       </c>
-      <c r="C39" s="5">
+      <c r="C39" s="4">
         <v>0.251</v>
       </c>
-      <c r="D39" s="5">
+      <c r="D39" s="4">
         <v>0.13800000000000001</v>
       </c>
-      <c r="E39" s="5">
+      <c r="E39" s="4">
         <v>0.25600000000000001</v>
       </c>
-      <c r="F39" s="5">
+      <c r="F39" s="4">
         <v>0.13600000000000001</v>
       </c>
-      <c r="G39" s="5">
+      <c r="G39" s="4">
         <v>0.25</v>
       </c>
-      <c r="H39" s="5">
+      <c r="H39" s="4">
         <v>0.14799999999999999</v>
       </c>
     </row>
     <row r="40" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A40" s="4">
+      <c r="A40" s="3">
         <v>5</v>
       </c>
-      <c r="B40" s="4">
+      <c r="B40" s="3">
         <v>3000</v>
       </c>
-      <c r="C40" s="5">
+      <c r="C40" s="4">
         <v>0.252</v>
       </c>
-      <c r="D40" s="5">
+      <c r="D40" s="4">
         <v>0.13600000000000001</v>
       </c>
-      <c r="E40" s="5">
+      <c r="E40" s="4">
         <v>0.25800000000000001</v>
       </c>
-      <c r="F40" s="5">
+      <c r="F40" s="4">
         <v>0.13400000000000001</v>
       </c>
-      <c r="G40" s="5">
+      <c r="G40" s="4">
         <v>0.25700000000000001</v>
       </c>
-      <c r="H40" s="5">
+      <c r="H40" s="4">
         <v>0.15</v>
       </c>
     </row>
     <row r="41" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A41" s="4">
+      <c r="A41" s="3">
         <v>5</v>
       </c>
-      <c r="B41" s="4">
+      <c r="B41" s="3">
         <v>4000</v>
       </c>
-      <c r="C41" s="5">
+      <c r="C41" s="4">
         <v>0.253</v>
       </c>
-      <c r="D41" s="5">
+      <c r="D41" s="4">
         <v>0.13700000000000001</v>
       </c>
-      <c r="E41" s="5">
+      <c r="E41" s="4">
         <v>0.26200000000000001</v>
       </c>
-      <c r="F41" s="5">
+      <c r="F41" s="4">
         <v>0.13500000000000001</v>
       </c>
-      <c r="G41" s="5">
+      <c r="G41" s="4">
         <v>0.251</v>
       </c>
-      <c r="H41" s="5">
+      <c r="H41" s="4">
         <v>0.14799999999999999</v>
       </c>
     </row>
     <row r="42" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A42" s="4">
+      <c r="A42" s="3">
         <v>5</v>
       </c>
-      <c r="B42" s="4">
+      <c r="B42" s="3">
         <v>5000</v>
       </c>
-      <c r="C42" s="5">
+      <c r="C42" s="4">
         <v>0.249</v>
       </c>
-      <c r="D42" s="5">
+      <c r="D42" s="4">
         <v>0.13800000000000001</v>
       </c>
-      <c r="E42" s="5">
+      <c r="E42" s="4">
         <v>0.255</v>
       </c>
-      <c r="F42" s="5">
+      <c r="F42" s="4">
         <v>0.13600000000000001</v>
       </c>
-      <c r="G42" s="5">
+      <c r="G42" s="4">
         <v>0.25</v>
       </c>
-      <c r="H42" s="5">
+      <c r="H42" s="4">
         <v>0.15</v>
       </c>
     </row>
     <row r="43" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A43" s="3">
+      <c r="A43" s="2">
         <v>6</v>
       </c>
-      <c r="B43" s="3">
+      <c r="B43" s="2">
         <v>250</v>
       </c>
-      <c r="C43" s="6">
+      <c r="C43" s="5">
         <v>0.22700000000000001</v>
       </c>
-      <c r="D43" s="6">
+      <c r="D43" s="5">
         <v>0.124</v>
       </c>
-      <c r="E43" s="6">
+      <c r="E43" s="5">
         <v>0.23499999999999999</v>
       </c>
-      <c r="F43" s="6">
+      <c r="F43" s="5">
         <v>0.127</v>
       </c>
-      <c r="G43" s="6">
+      <c r="G43" s="5">
         <v>0.22900000000000001</v>
       </c>
-      <c r="H43" s="6">
+      <c r="H43" s="5">
         <v>0.128</v>
       </c>
     </row>
     <row r="44" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A44" s="3">
+      <c r="A44" s="2">
         <v>6</v>
       </c>
-      <c r="B44" s="3">
+      <c r="B44" s="2">
         <v>500</v>
       </c>
-      <c r="C44" s="6">
+      <c r="C44" s="5">
         <v>0.22600000000000001</v>
       </c>
-      <c r="D44" s="6">
+      <c r="D44" s="5">
         <v>0.122</v>
       </c>
-      <c r="E44" s="6">
+      <c r="E44" s="5">
         <v>0.23300000000000001</v>
       </c>
-      <c r="F44" s="6">
+      <c r="F44" s="5">
         <v>0.125</v>
       </c>
-      <c r="G44" s="6">
+      <c r="G44" s="5">
         <v>0.22700000000000001</v>
       </c>
-      <c r="H44" s="6">
+      <c r="H44" s="5">
         <v>0.125</v>
       </c>
     </row>
     <row r="45" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A45" s="3">
+      <c r="A45" s="2">
         <v>6</v>
       </c>
-      <c r="B45" s="3">
+      <c r="B45" s="2">
         <v>750</v>
       </c>
-      <c r="C45" s="6">
+      <c r="C45" s="5">
         <v>0.22500000000000001</v>
       </c>
-      <c r="D45" s="6">
+      <c r="D45" s="5">
         <v>0.11899999999999999</v>
       </c>
-      <c r="E45" s="6">
+      <c r="E45" s="5">
         <v>0.23200000000000001</v>
       </c>
-      <c r="F45" s="6">
+      <c r="F45" s="5">
         <v>0.12</v>
       </c>
-      <c r="G45" s="6">
+      <c r="G45" s="5">
         <v>0.22700000000000001</v>
       </c>
-      <c r="H45" s="6">
+      <c r="H45" s="5">
         <v>0.124</v>
       </c>
     </row>
     <row r="46" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A46" s="3">
+      <c r="A46" s="2">
         <v>6</v>
       </c>
-      <c r="B46" s="3">
+      <c r="B46" s="2">
         <v>1000</v>
       </c>
-      <c r="C46" s="6">
+      <c r="C46" s="5">
         <v>0.22600000000000001</v>
       </c>
-      <c r="D46" s="6">
+      <c r="D46" s="5">
         <v>0.121</v>
       </c>
-      <c r="E46" s="6">
+      <c r="E46" s="5">
         <v>0.23300000000000001</v>
       </c>
-      <c r="F46" s="6">
+      <c r="F46" s="5">
         <v>0.122</v>
       </c>
-      <c r="G46" s="6">
+      <c r="G46" s="5">
         <v>0.22700000000000001</v>
       </c>
-      <c r="H46" s="6">
+      <c r="H46" s="5">
         <v>0.126</v>
       </c>
     </row>
     <row r="47" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A47" s="3">
+      <c r="A47" s="2">
         <v>6</v>
       </c>
-      <c r="B47" s="3">
+      <c r="B47" s="2">
         <v>2000</v>
       </c>
-      <c r="C47" s="6">
+      <c r="C47" s="5">
         <v>0.22500000000000001</v>
       </c>
-      <c r="D47" s="6">
+      <c r="D47" s="5">
         <v>0.123</v>
       </c>
-      <c r="E47" s="6">
+      <c r="E47" s="5">
         <v>0.23200000000000001</v>
       </c>
-      <c r="F47" s="6">
+      <c r="F47" s="5">
         <v>0.123</v>
       </c>
-      <c r="G47" s="6">
+      <c r="G47" s="5">
         <v>0.22600000000000001</v>
       </c>
-      <c r="H47" s="6">
+      <c r="H47" s="5">
         <v>0.127</v>
       </c>
     </row>
     <row r="48" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A48" s="3">
+      <c r="A48" s="2">
         <v>6</v>
       </c>
-      <c r="B48" s="3">
+      <c r="B48" s="2">
         <v>3000</v>
       </c>
-      <c r="C48" s="6">
+      <c r="C48" s="5">
         <v>0.22600000000000001</v>
       </c>
-      <c r="D48" s="6">
+      <c r="D48" s="5">
         <v>0.12</v>
       </c>
-      <c r="E48" s="6">
+      <c r="E48" s="5">
         <v>0.23400000000000001</v>
       </c>
-      <c r="F48" s="6">
+      <c r="F48" s="5">
         <v>0.121</v>
       </c>
-      <c r="G48" s="6">
+      <c r="G48" s="5">
         <v>0.22700000000000001</v>
       </c>
-      <c r="H48" s="6">
+      <c r="H48" s="5">
         <v>0.126</v>
       </c>
     </row>
     <row r="49" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A49" s="3">
+      <c r="A49" s="2">
         <v>6</v>
       </c>
-      <c r="B49" s="3">
+      <c r="B49" s="2">
         <v>4000</v>
       </c>
-      <c r="C49" s="6">
+      <c r="C49" s="5">
         <v>0.22500000000000001</v>
       </c>
-      <c r="D49" s="6">
+      <c r="D49" s="5">
         <v>0.124</v>
       </c>
-      <c r="E49" s="6">
+      <c r="E49" s="5">
         <v>0.23200000000000001</v>
       </c>
-      <c r="F49" s="6">
+      <c r="F49" s="5">
         <v>0.125</v>
       </c>
-      <c r="G49" s="6">
+      <c r="G49" s="5">
         <v>0.22600000000000001</v>
       </c>
-      <c r="H49" s="6">
+      <c r="H49" s="5">
         <v>0.127</v>
       </c>
     </row>
     <row r="50" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A50" s="3">
+      <c r="A50" s="2">
         <v>6</v>
       </c>
-      <c r="B50" s="3">
+      <c r="B50" s="2">
         <v>5000</v>
       </c>
-      <c r="C50" s="6">
+      <c r="C50" s="5">
         <v>0.22500000000000001</v>
       </c>
-      <c r="D50" s="6">
+      <c r="D50" s="5">
         <v>0.12</v>
       </c>
-      <c r="E50" s="6">
+      <c r="E50" s="5">
         <v>0.23100000000000001</v>
       </c>
-      <c r="F50" s="6">
+      <c r="F50" s="5">
         <v>0.121</v>
       </c>
-      <c r="G50" s="6">
+      <c r="G50" s="5">
         <v>0.22600000000000001</v>
       </c>
-      <c r="H50" s="6">
+      <c r="H50" s="5">
         <v>0.125</v>
       </c>
     </row>
     <row r="51" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A51" s="4">
+      <c r="A51" s="3">
         <v>7</v>
       </c>
-      <c r="B51" s="4">
+      <c r="B51" s="3">
         <v>250</v>
       </c>
-      <c r="C51" s="5">
+      <c r="C51" s="4">
         <v>0.23100000000000001</v>
       </c>
-      <c r="D51" s="5">
+      <c r="D51" s="4">
         <v>0.121</v>
       </c>
-      <c r="E51" s="5">
+      <c r="E51" s="4">
         <v>0.23699999999999999</v>
       </c>
-      <c r="F51" s="5">
+      <c r="F51" s="4">
         <v>0.12</v>
       </c>
-      <c r="G51" s="5">
+      <c r="G51" s="4">
         <v>0.23400000000000001</v>
       </c>
-      <c r="H51" s="5">
+      <c r="H51" s="4">
         <v>0.13</v>
       </c>
     </row>
     <row r="52" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A52" s="4">
+      <c r="A52" s="3">
         <v>7</v>
       </c>
-      <c r="B52" s="4">
+      <c r="B52" s="3">
         <v>500</v>
       </c>
-      <c r="C52" s="5">
+      <c r="C52" s="4">
         <v>0.22800000000000001</v>
       </c>
-      <c r="D52" s="5">
+      <c r="D52" s="4">
         <v>0.128</v>
       </c>
-      <c r="E52" s="5">
+      <c r="E52" s="4">
         <v>0.23699999999999999</v>
       </c>
-      <c r="F52" s="5">
+      <c r="F52" s="4">
         <v>0.13</v>
       </c>
-      <c r="G52" s="5">
+      <c r="G52" s="4">
         <v>0.23100000000000001</v>
       </c>
-      <c r="H52" s="5">
+      <c r="H52" s="4">
         <v>0.129</v>
       </c>
     </row>
     <row r="53" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A53" s="4">
+      <c r="A53" s="3">
         <v>7</v>
       </c>
-      <c r="B53" s="4">
+      <c r="B53" s="3">
         <v>750</v>
       </c>
-      <c r="C53" s="5">
+      <c r="C53" s="4">
         <v>0.23</v>
       </c>
-      <c r="D53" s="5">
+      <c r="D53" s="4">
         <v>0.124</v>
       </c>
-      <c r="E53" s="5">
+      <c r="E53" s="4">
         <v>0.23599999999999999</v>
       </c>
-      <c r="F53" s="5">
+      <c r="F53" s="4">
         <v>0.128</v>
       </c>
-      <c r="G53" s="5">
+      <c r="G53" s="4">
         <v>0.23200000000000001</v>
       </c>
-      <c r="H53" s="5">
+      <c r="H53" s="4">
         <v>0.129</v>
       </c>
     </row>
     <row r="54" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A54" s="4">
+      <c r="A54" s="3">
         <v>7</v>
       </c>
-      <c r="B54" s="4">
+      <c r="B54" s="3">
         <v>1000</v>
       </c>
-      <c r="C54" s="5">
+      <c r="C54" s="4">
         <v>0.23100000000000001</v>
       </c>
-      <c r="D54" s="5">
+      <c r="D54" s="4">
         <v>0.129</v>
       </c>
-      <c r="E54" s="5">
+      <c r="E54" s="4">
         <v>0.23799999999999999</v>
       </c>
-      <c r="F54" s="5">
+      <c r="F54" s="4">
         <v>0.13</v>
       </c>
-      <c r="G54" s="5">
+      <c r="G54" s="4">
         <v>0.23499999999999999</v>
       </c>
-      <c r="H54" s="5">
+      <c r="H54" s="4">
         <v>0.13200000000000001</v>
       </c>
     </row>
     <row r="55" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A55" s="4">
+      <c r="A55" s="3">
         <v>7</v>
       </c>
-      <c r="B55" s="4">
+      <c r="B55" s="3">
         <v>2000</v>
       </c>
-      <c r="C55" s="5">
+      <c r="C55" s="4">
         <v>0.23</v>
       </c>
-      <c r="D55" s="5">
+      <c r="D55" s="4">
         <v>0.125</v>
       </c>
-      <c r="E55" s="5">
+      <c r="E55" s="4">
         <v>0.23899999999999999</v>
       </c>
-      <c r="F55" s="5">
+      <c r="F55" s="4">
         <v>0.126</v>
       </c>
-      <c r="G55" s="5">
+      <c r="G55" s="4">
         <v>0.23599999999999999</v>
       </c>
-      <c r="H55" s="5">
+      <c r="H55" s="4">
         <v>0.13200000000000001</v>
       </c>
     </row>
     <row r="56" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A56" s="4">
+      <c r="A56" s="3">
         <v>7</v>
       </c>
-      <c r="B56" s="4">
+      <c r="B56" s="3">
         <v>3000</v>
       </c>
-      <c r="C56" s="5">
+      <c r="C56" s="4">
         <v>0.22600000000000001</v>
       </c>
-      <c r="D56" s="5">
+      <c r="D56" s="4">
         <v>0.126</v>
       </c>
-      <c r="E56" s="5">
+      <c r="E56" s="4">
         <v>0.23499999999999999</v>
       </c>
-      <c r="F56" s="5">
+      <c r="F56" s="4">
         <v>0.128</v>
       </c>
-      <c r="G56" s="5">
+      <c r="G56" s="4">
         <v>0.22900000000000001</v>
       </c>
-      <c r="H56" s="5">
+      <c r="H56" s="4">
         <v>0.129</v>
       </c>
     </row>
     <row r="57" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A57" s="4">
+      <c r="A57" s="3">
         <v>7</v>
       </c>
-      <c r="B57" s="4">
+      <c r="B57" s="3">
         <v>4000</v>
       </c>
-      <c r="C57" s="5">
+      <c r="C57" s="4">
         <v>0.221</v>
       </c>
-      <c r="D57" s="5">
+      <c r="D57" s="4">
         <v>0.123</v>
       </c>
-      <c r="E57" s="5">
+      <c r="E57" s="4">
         <v>0.22600000000000001</v>
       </c>
-      <c r="F57" s="5">
+      <c r="F57" s="4">
         <v>0.122</v>
       </c>
-      <c r="G57" s="5">
+      <c r="G57" s="4">
         <v>0.223</v>
       </c>
-      <c r="H57" s="5">
+      <c r="H57" s="4">
         <v>0.13200000000000001</v>
       </c>
     </row>
     <row r="58" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A58" s="4">
+      <c r="A58" s="3">
         <v>7</v>
       </c>
-      <c r="B58" s="4">
+      <c r="B58" s="3">
         <v>5000</v>
       </c>
-      <c r="C58" s="5">
+      <c r="C58" s="4">
         <v>0.22600000000000001</v>
       </c>
-      <c r="D58" s="5">
+      <c r="D58" s="4">
         <v>0.127</v>
       </c>
-      <c r="E58" s="5">
+      <c r="E58" s="4">
         <v>0.23599999999999999</v>
       </c>
-      <c r="F58" s="5">
+      <c r="F58" s="4">
         <v>0.127</v>
       </c>
-      <c r="G58" s="5">
+      <c r="G58" s="4">
         <v>0.22800000000000001</v>
       </c>
-      <c r="H58" s="5">
+      <c r="H58" s="4">
         <v>0.13300000000000001</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="5">
+  <mergeCells count="6">
+    <mergeCell ref="L1:N1"/>
     <mergeCell ref="C1:D1"/>
     <mergeCell ref="E1:F1"/>
     <mergeCell ref="G1:H1"/>

</xml_diff>